<commit_message>
Cambio en el nombre de archivo y actualizar resultados
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\El Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D641FAE-1C36-4675-8E04-858DE5EF9943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E41A3E-DB9C-45A0-90F7-8D59AA6D3767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FA68BC49-A0B4-45D9-976E-79E5F52D2F97}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$3:$E$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$2:$E$10</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="36">
   <si>
     <t>RESULTADOS DEL PROGRAMA</t>
   </si>
@@ -141,6 +141,12 @@
   </si>
   <si>
     <t>Raptors</t>
+  </si>
+  <si>
+    <t>Kings</t>
+  </si>
+  <si>
+    <t>Pacers</t>
   </si>
 </sst>
 </file>
@@ -180,23 +186,21 @@
     </font>
     <font>
       <i/>
-      <u/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="14"/>
       <color theme="6" tint="-0.249977111117893"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,6 +216,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -237,17 +247,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -260,29 +264,251 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="13">
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.749992370372631"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -311,6 +537,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}" name="Tabla2" displayName="Tabla2" ref="A2:E26" totalsRowShown="0" headerRowDxfId="3" dataDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="A2:E26" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{0E447FFE-76DF-40D6-9B41-5A9BD26FD310}" name="Fecha" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{DE6DE503-5A73-4772-8C8C-CA7907C32390}" name="Casa" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{A1100241-296B-4835-A91E-5F599728700C}" name="Visitante" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{DFF2B1DE-CB62-4759-A466-8869F8A4603D}" name="Programa" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{ADEE255F-5BE1-4631-A79B-1A9E0D02464B}" name="Final" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -630,16 +870,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD7988D-F199-445A-9D79-79373189F41A}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="19.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
@@ -652,282 +893,398 @@
       <c r="E1" s="13"/>
     </row>
     <row r="2" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="A2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
+      <c r="A3" s="2">
+        <v>45359</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>45359</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>45359</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>45359</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>45359</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>45359</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
+        <v>45359</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="6">
+        <v>45359</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>45360</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>45360</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>45360</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>45360</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>45360</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>45360</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="6">
+        <v>45360</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="11"/>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="E20" s="12"/>
+    </row>
+    <row r="21" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
-        <v>45359</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="12"/>
+    </row>
+    <row r="22" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="12"/>
+    </row>
+    <row r="23" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
-        <v>45359</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="D23" s="11"/>
+      <c r="E23" s="12"/>
+    </row>
+    <row r="24" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24" s="11"/>
+      <c r="E24" s="12"/>
+    </row>
+    <row r="25" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A25" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B25" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C25" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="11"/>
+      <c r="E25" s="12"/>
+    </row>
+    <row r="26" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>45361</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
-        <v>45359</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
-        <v>45359</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
-        <v>45359</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
-        <v>45359</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
-        <v>45359</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E13" s="6"/>
-    </row>
-    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E15" s="6"/>
-    </row>
-    <row r="16" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="6"/>
-    </row>
-    <row r="17" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="6"/>
-    </row>
-    <row r="18" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
-        <v>45360</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="6"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E4:E18">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>$D4</formula>
+  <conditionalFormatting sqref="E3:E26">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+      <formula>$D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
-      <formula>$D4</formula>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+      <formula>$D3</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>